<commit_message>
7.1 Ajustes de la propuesta
</commit_message>
<xml_diff>
--- a/basesDatos/Bases de datos.xlsx
+++ b/basesDatos/Bases de datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\dauruxu\basesDatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ronald Fernando\dauruxu\basesDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34B73E3D-C159-4DDA-90CD-5D8745A1F523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90752975-9405-441C-ACBC-5A36B49B6018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4CEA32E9-E774-444D-8AB5-ED43118B390E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CEA32E9-E774-444D-8AB5-ED43118B390E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -649,22 +649,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13364D74-FB97-4AE3-BCDA-D11D9B800FC7}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -705,7 +705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -746,7 +746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -784,7 +784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -801,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -818,7 +818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -860,7 +860,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1010,7 +1010,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1052,7 +1052,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1088,7 +1088,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1109,7 +1109,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1384,18 +1384,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1418,14 +1418,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBD4A8D3-B3CD-4243-907B-6DF88FDCFB9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E70F1340-0C2E-4C28-BD65-C5027CD7E177}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1440,4 +1432,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBD4A8D3-B3CD-4243-907B-6DF88FDCFB9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>